<commit_message>
updates notebook 3 to eiv3.11
</commit_message>
<xml_diff>
--- a/Course-material-bw25/test_db_excel_w_ecoinvent.xlsx
+++ b/Course-material-bw25/test_db_excel_w_ecoinvent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/massimo/Documents/AAU/Teaching/Courses/2023/Module2/Course-material/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/massimo/Documents/AAU/Teaching/Courses/2025/2025-Advanced-LCA/Module2/Course-material-bw25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A328A070-4630-2F45-81D1-C37A9AF8011E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA601875-962F-8D45-89F3-6C2427410433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27740" windowHeight="18420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test0" sheetId="1" r:id="rId1"/>
@@ -105,18 +105,12 @@
     <t>False</t>
   </si>
   <si>
-    <t>biosphere3</t>
-  </si>
-  <si>
     <t>349b29d1-3e58-4c66-98b9-9d1a076efd2e</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>﻿'diesel production, low-sulfur' (kilogram, Europe without Switzerland, None)</t>
-  </si>
-  <si>
     <t>kilogram</t>
   </si>
   <si>
@@ -129,10 +123,16 @@
     <t>kilowatt hour</t>
   </si>
   <si>
-    <t>ecoinvent 3.9 conseq</t>
-  </si>
-  <si>
-    <t>cea1e434115aa84cbfd7dc3086b61e80</t>
+    <t>ecoinvent-3.11-biosphere</t>
+  </si>
+  <si>
+    <t>5e00f9695a7ce345a4a17c517fd1ea62</t>
+  </si>
+  <si>
+    <t>ecoinvent-3.11-consequential</t>
+  </si>
+  <si>
+    <t>diesel production, low-sulfur' (kilogram, CH, None)</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,12 +520,12 @@
         <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -534,13 +534,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>5</v>
@@ -549,7 +549,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -566,13 +566,13 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>0</v>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>1</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -610,22 +610,22 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>3</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -657,13 +657,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>4</v>
@@ -672,7 +672,7 @@
         <v>0.1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>3</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -701,13 +701,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>0</v>
@@ -716,7 +716,7 @@
         <v>100</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>6</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -733,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
@@ -742,24 +742,24 @@
         <v>33</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H7">
         <v>100</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O7" t="s">
-        <v>28</v>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -768,22 +768,22 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="H8">
         <v>10</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>3</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
@@ -800,13 +800,13 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>4</v>
@@ -815,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>3</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -832,13 +832,13 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>7</v>
@@ -847,7 +847,7 @@
         <v>-50</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>3</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -864,7 +864,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>3</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
@@ -881,7 +881,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>3</v>

</xml_diff>